<commit_message>
Added all documentation for Sprint 4
</commit_message>
<xml_diff>
--- a/Documentation/BIKERR Risk Tracking Spreadsheet.xlsx
+++ b/Documentation/BIKERR Risk Tracking Spreadsheet.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
-    <t>Risk Tracking Spreadsheet 1.2</t>
+    <t>Risk Tracking Spreadsheet 1.3</t>
   </si>
   <si>
     <t>RISK DESCRIPTION</t>
@@ -112,7 +112,7 @@
     <t>User enters invalid data that is accepted into certain inputs potentially corrupting the data base and also of displaying false information.</t>
   </si>
   <si>
-    <t xml:space="preserve">Make sure that all inputs have validation tests to insure only valid information is snet tot he back-end. </t>
+    <t>git checkout</t>
   </si>
   <si>
     <t xml:space="preserve">Shashank Patel </t>

</xml_diff>